<commit_message>
Shifted progress to SQL Server
</commit_message>
<xml_diff>
--- a/classicmodels_sql_tracker.xlsx
+++ b/classicmodels_sql_tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Desktop\SQL Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Desktop\SQL Learning\sql_learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2456EB27-33FC-45A6-8C89-DEAB0B4AFD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3313D31F-154C-4566-BFF6-CD111D7DA76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8328" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8340" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="85">
   <si>
     <t>Category</t>
   </si>
@@ -648,7 +648,7 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,6 +873,9 @@
       <c r="C15" t="s">
         <v>26</v>
       </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">

</xml_diff>